<commit_message>
added correlated polling errors
</commit_message>
<xml_diff>
--- a/modell/Largest remainder.xlsx
+++ b/modell/Largest remainder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruker/Documents/Programmering/2024/valgside/valgmodell/modell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD112A6-E7E9-E549-AEDA-E0E5868974D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00C8838-2AA7-284D-A500-E3C7021853DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="720" windowWidth="28040" windowHeight="17040" xr2:uid="{99E4D808-A91A-6C4D-949D-4D9973E2D857}"/>
+    <workbookView xWindow="3600" yWindow="2160" windowWidth="13060" windowHeight="14940" xr2:uid="{99E4D808-A91A-6C4D-949D-4D9973E2D857}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>RS</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>REM</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>FRP</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>KRF</t>
+  </si>
+  <si>
+    <t>MDG</t>
   </si>
 </sst>
 </file>
@@ -45,7 +60,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -87,9 +102,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,26 +468,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1EFF4C-4BA9-4748-AF3B-93F5B36AE672}">
-  <dimension ref="D3:J13"/>
+  <dimension ref="C3:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="3" spans="4:10">
+    <row r="3" spans="3:10">
       <c r="D3">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="4:10">
+    <row r="4" spans="3:10">
       <c r="J4">
         <f>47000/100000*11</f>
         <v>5.17</v>
       </c>
     </row>
-    <row r="5" spans="4:10">
+    <row r="5" spans="3:10">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -486,21 +501,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:10">
+    <row r="6" spans="3:10">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
       <c r="D6">
-        <v>40</v>
+        <v>54.2</v>
       </c>
       <c r="E6" s="3">
         <f>D6/$D$13*$D$3</f>
-        <v>40</v>
+        <v>64.099370188943325</v>
       </c>
       <c r="F6" s="3">
         <f>ROUNDDOWN(E6,0)</f>
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2">
         <f>E6-F6</f>
-        <v>0</v>
+        <v>9.9370188943325388E-2</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -509,136 +527,148 @@
         <v>1</v>
       </c>
       <c r="J6" s="3">
-        <f>I6+F6</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10">
+        <f t="shared" ref="J6:J12" si="0">I6+F6</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
       <c r="D7">
-        <v>28</v>
+        <v>42.5</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7:E12" si="0">D7/$D$13*$D$3</f>
-        <v>28.000000000000004</v>
+        <f t="shared" ref="E7:E12" si="1">D7/$D$13*$D$3</f>
+        <v>50.262421273617925</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F12" si="1">ROUNDDOWN(E7,0)</f>
-        <v>28</v>
+        <f t="shared" ref="F7:F12" si="2">ROUNDDOWN(E7,0)</f>
+        <v>50</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ref="G7:G12" si="2">E7-F7</f>
-        <v>0</v>
+        <f t="shared" ref="G7:G12" si="3">E7-F7</f>
+        <v>0.26242127361792456</v>
       </c>
       <c r="J7" s="3">
-        <f>I7+F7</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="4:10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
       <c r="D8">
-        <v>57</v>
+        <v>27.4</v>
       </c>
       <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>32.404478656403086</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.40447865640308578</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="F8" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
         <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-      <c r="G8" s="2">
+        <v>2.3652904128761376</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.36529041287613762</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.94611616515045505</v>
+      </c>
+      <c r="F10" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3">
-        <f>I8+F8</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10">
-      <c r="D9">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="G10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.94611616515045505</v>
+      </c>
+      <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F9" s="3">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J9" s="3">
-        <f>I9+F9</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10">
-      <c r="D10">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F10" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="3">
-        <f>I10+F10</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10">
+    </row>
+    <row r="11" spans="3:10">
       <c r="D11">
         <v>8</v>
       </c>
       <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>9.4611616515045505</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.46116165150455046</v>
+      </c>
+      <c r="J11" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="F11" s="3">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="3">
-        <f>I11+F11</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10">
       <c r="D12">
         <v>8</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>9.4611616515045505</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.46116165150455046</v>
       </c>
       <c r="H12">
         <v>3</v>
@@ -647,14 +677,14 @@
         <v>1</v>
       </c>
       <c r="J12" s="3">
-        <f>I12+F12</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="4:10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10">
       <c r="D13" s="1">
         <f>SUM(D6:D12)</f>
-        <v>169</v>
+        <v>142.89999999999998</v>
       </c>
       <c r="E13" s="1">
         <f>SUM(E6:E12)</f>
@@ -662,15 +692,15 @@
       </c>
       <c r="F13" s="1">
         <f>SUM(F6:F12)</f>
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G13" s="4">
         <f>SUM(G6:G12)</f>
-        <v>0</v>
+        <v>3.0000000000000293</v>
       </c>
       <c r="J13" s="1">
         <f>SUM(J6:J12)</f>
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>